<commit_message>
Agregue mensaje para equipo registrado y filtro para que no aparezca uno mismo como opcion en tagsinput
</commit_message>
<xml_diff>
--- a/Seguimiento.xlsx
+++ b/Seguimiento.xlsx
@@ -441,7 +441,7 @@
   <dimension ref="A1:D199"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="28.5" x14ac:dyDescent="0.45"/>
@@ -476,6 +476,9 @@
       <c r="B3" s="2">
         <v>43278</v>
       </c>
+      <c r="C3" s="2">
+        <v>43279</v>
+      </c>
       <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:4" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="1.35">
@@ -484,6 +487,9 @@
       </c>
       <c r="B4" s="2">
         <v>43278</v>
+      </c>
+      <c r="C4" s="2">
+        <v>43279</v>
       </c>
       <c r="D4" s="6"/>
     </row>

</xml_diff>